<commit_message>
Agrego cargas de reparación en techo Lr
</commit_message>
<xml_diff>
--- a/Tarea 03/diseño corte.xlsx
+++ b/Tarea 03/diseño corte.xlsx
@@ -5,35 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Diseño de Albañileria Estructural\proyecto-CI5223\Tarea 03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA94A4-B67C-436C-BDA6-6F551233E4BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F9D826-45D9-4CFC-85A2-830447944756}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="4596" activeTab="2" xr2:uid="{3C432B30-B9EB-47E7-B497-33C5C308436F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4590" activeTab="1" xr2:uid="{3C432B30-B9EB-47E7-B497-33C5C308436F}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistencia al corte" sheetId="1" r:id="rId1"/>
     <sheet name="Solicitación timpano" sheetId="2" r:id="rId2"/>
     <sheet name="Solicitacion cercha madera" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Pier</t>
   </si>
@@ -122,15 +117,6 @@
     <t>$\rho_{cad} \quad (tonf/m^3)$</t>
   </si>
   <si>
-    <t>$Q_{timp} \quad (tonf/m)$</t>
-  </si>
-  <si>
-    <t>$Q_{cad} \quad (tonf/m)$</t>
-  </si>
-  <si>
-    <t>$Q_{total} \quad (tonf/m)$</t>
-  </si>
-  <si>
     <t>Propiedades madera</t>
   </si>
   <si>
@@ -183,6 +169,27 @@
   </si>
   <si>
     <t>Solicitaciones a aplicar en ETABS</t>
+  </si>
+  <si>
+    <t>$Q_{timp} \quad (kgf/m)$</t>
+  </si>
+  <si>
+    <t>$Q_{cad} \quad (kgf/m)$</t>
+  </si>
+  <si>
+    <t>$Q_{total} \quad (kgf/m)$</t>
+  </si>
+  <si>
+    <t>L_r (kgf)</t>
+  </si>
+  <si>
+    <t>$A_{trib.cost} [m^2]$</t>
+  </si>
+  <si>
+    <t>$P_{L_r} \quad (kgf)$</t>
+  </si>
+  <si>
+    <t>$Q_{L_r} \quad (kgf/m)$</t>
   </si>
 </sst>
 </file>
@@ -190,9 +197,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -381,61 +388,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -459,13 +466,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -507,15 +514,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -555,13 +562,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
@@ -603,14 +610,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>261228</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>548791</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>339241</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>94857</xdr:rowOff>
     </xdr:to>
@@ -649,7 +656,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -951,64 +958,64 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="23">
         <v>3.8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="23">
         <v>14000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="23">
         <v>2.7708847204661971E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="23">
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>0.25341665296503307</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1026,12 +1033,12 @@
         <v>0.11696153213770756</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1047,7 @@
         <v>0.33139100772350477</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1056,7 @@
         <v>0.25341665296503307</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7">
         <v>-2.4980000000000002</v>
@@ -1124,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7">
         <v>-2.4980000000000002</v>
@@ -1164,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7">
         <v>-2.4980000000000002</v>
@@ -1204,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7">
         <v>-2.4980000000000002</v>
@@ -1244,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7">
         <v>-2.4980000000000002</v>
@@ -1284,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7">
         <v>-2.4980000000000002</v>
@@ -1324,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7">
         <v>-2.4980000000000002</v>
@@ -1364,7 +1371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7">
         <v>-2.4980000000000002</v>
@@ -1404,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7">
         <v>-2.4980000000000002</v>
@@ -1444,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7">
         <v>-2.4980000000000002</v>
@@ -1484,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7">
         <v>-2.4980000000000002</v>
@@ -1524,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7">
         <v>-2.4980000000000002</v>
@@ -1564,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7">
         <v>-2.4980000000000002</v>
@@ -1604,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7">
         <v>-2.4980000000000002</v>
@@ -1644,65 +1651,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1711,26 +1718,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C85F50-745A-40AF-AD65-075F51DE0E61}">
-  <dimension ref="B2:C17"/>
+  <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="6"/>
-    <col min="2" max="2" width="26.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.5546875" style="6"/>
+    <col min="1" max="1" width="7.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1745,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
@@ -1746,7 +1753,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1754,21 +1761,21 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="8">
-        <v>8.39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>28</v>
       </c>
@@ -1776,7 +1783,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1784,7 +1791,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1792,7 +1799,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1800,31 +1807,40 @@
         <v>10.49</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C15" s="8">
-        <f>C3*C4*C5</f>
-        <v>0.26208000000000009</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+        <f>C3*C4*C5*1000</f>
+        <v>262.0800000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C16" s="8">
-        <f>C9*C10*C11</f>
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="12">
-        <f>C15+C16</f>
-        <v>0.30408000000000007</v>
+        <f>C9*C10*C11*1000</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="11">
+        <f>C15+C16+'Solicitacion cercha madera'!C27*'Solicitacion cercha madera'!C10/'Solicitación timpano'!C6</f>
+        <v>307.01562500000011</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6">
+        <f>'Solicitacion cercha madera'!F22/2*5/'Solicitación timpano'!C6</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1839,303 +1855,355 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799F4323-B58A-4472-B8A9-BF42EC749805}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="B1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.5546875" style="6"/>
+    <col min="1" max="1" width="8.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5703125" style="6"/>
+    <col min="5" max="5" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="14"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="8">
+        <v>550</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="8">
+        <v>50</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.157</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="19"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="8">
-        <v>550</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="19"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="C11" s="8">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="8">
+        <f>C11*C5/1000*C4/1000</f>
+        <v>4.2699999999999995E-2</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="20"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="8">
+        <f>C11/10</f>
+        <v>0.85399999999999987</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="8">
-        <v>100</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="19"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="C16" s="8">
+        <f>C15*C5/1000*C4/1000</f>
+        <v>4.2699999999999995E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="6">
+        <v>49.59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="E19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="6">
+        <f>8.4/5*5/6</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="H19" s="6">
+        <f>10*8.4</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="8">
+        <f>C3*C8/2</f>
+        <v>43.174999999999997</v>
+      </c>
+      <c r="H20" s="6">
+        <f>H18/H19</f>
+        <v>0.59035714285714291</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="25">
+        <f>$C$16*$C$3*2*5/2</f>
+        <v>11.742499999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="25">
+        <f>C16*C3*5/2</f>
+        <v>5.871249999999999</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.157</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="8">
-        <v>5</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="8">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="8">
-        <f>B12*B6/1000*B5/1000</f>
-        <v>4.2699999999999995E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="8">
-        <f>B12/8</f>
-        <v>1.0674999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="8">
-        <f>B16*B6/1000*B5/1000</f>
-        <v>5.3374999999999994E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="13"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="F22" s="25">
+        <f>F19*100</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="27"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="8">
-        <f>B4*B9/2</f>
-        <v>43.174999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="C26" s="25">
+        <f>C20+C21</f>
+        <v>54.917499999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="27">
-        <f>B17*B4*2*5/2</f>
-        <v>14.678124999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="27">
-        <f>B17*B4*5/2</f>
-        <v>7.3390624999999989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="13"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="27">
-        <f>B21+B22</f>
-        <v>57.853124999999991</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="27">
-        <f>B23</f>
-        <v>7.3390624999999989</v>
+      <c r="C27" s="25">
+        <f>C22</f>
+        <v>5.871249999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="25">
+        <f>+F22*C10/2</f>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44941632-0BEC-43CE-AA79-0E3620F1F440}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglo cargas de reparación de uso de techo
</commit_message>
<xml_diff>
--- a/Tarea 03/diseño corte.xlsx
+++ b/Tarea 03/diseño corte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ramos Ingenieria\12° Semestre\Diseño de Albañileria Estructural\proyecto-CI5223\Tarea 03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F9D826-45D9-4CFC-85A2-830447944756}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6834EAD2-F7B4-4B09-AEBB-94BF1458EFD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4590" activeTab="1" xr2:uid="{3C432B30-B9EB-47E7-B497-33C5C308436F}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -443,6 +443,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1721,7 +1724,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,8 +1842,8 @@
         <v>53</v>
       </c>
       <c r="C18" s="6">
-        <f>'Solicitacion cercha madera'!F22/2*5/'Solicitación timpano'!C6</f>
-        <v>35</v>
+        <f>'Solicitacion cercha madera'!F22/2*5/C6</f>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1857,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799F4323-B58A-4472-B8A9-BF42EC749805}">
   <dimension ref="B1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,9 +2106,9 @@
       <c r="E19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="6">
-        <f>8.4/5*5/6</f>
-        <v>1.4000000000000001</v>
+      <c r="F19" s="28">
+        <f>8.4/5*10/6</f>
+        <v>2.8000000000000003</v>
       </c>
       <c r="H19" s="6">
         <f>10*8.4</f>
@@ -2147,7 +2150,7 @@
       </c>
       <c r="F22" s="25">
         <f>F19*100</f>
-        <v>140</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -2179,8 +2182,8 @@
         <v>52</v>
       </c>
       <c r="C28" s="25">
-        <f>+F22*C10/2</f>
-        <v>350</v>
+        <f>+F22*6/2</f>
+        <v>840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avance 2 diseño al corte
</commit_message>
<xml_diff>
--- a/Tarea 03/diseño corte.xlsx
+++ b/Tarea 03/diseño corte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto albañilería\proyecto-CI5223\Tarea 03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC56FA5-AB6F-4F6F-BD51-E089C1158011}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1454E1A2-35E1-4CAD-BAD8-CB6A745CDB38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="4596" activeTab="1" xr2:uid="{3C432B30-B9EB-47E7-B497-33C5C308436F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="4596" activeTab="2" xr2:uid="{3C432B30-B9EB-47E7-B497-33C5C308436F}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados por pier" sheetId="5" r:id="rId1"/>
@@ -50,33 +50,6 @@
     <t>Caso 1: Sin considerar armadura de corte</t>
   </si>
   <si>
-    <t>$V_2 \quad (tonf)$</t>
-  </si>
-  <si>
-    <t>$M_3 \quad (tonf \cdot m)$</t>
-  </si>
-  <si>
-    <t>$d \quad (m)$</t>
-  </si>
-  <si>
-    <t>$\tau_{0} \quad (tonf/m^2)$</t>
-  </si>
-  <si>
-    <t>$\tau_{1} \quad (tonf/m^2)$</t>
-  </si>
-  <si>
-    <t>$\tau_{sol} \quad (tonf/m^2)$</t>
-  </si>
-  <si>
-    <t>$M/Vd \quad (-)$</t>
-  </si>
-  <si>
-    <t>$\rho_h \quad (-)$</t>
-  </si>
-  <si>
-    <t>$f'm \quad (MPa)$</t>
-  </si>
-  <si>
     <t>$M/Vd=0 $</t>
   </si>
   <si>
@@ -86,18 +59,6 @@
     <t>Caso 2: Armadura resiste todo el corte</t>
   </si>
   <si>
-    <t>$b \quad (m)$</t>
-  </si>
-  <si>
-    <t>$F_s \quad (Mpa)$</t>
-  </si>
-  <si>
-    <t>$A_{esc} \quad (m^2)$</t>
-  </si>
-  <si>
-    <t>$Escantillon \quad (m)$</t>
-  </si>
-  <si>
     <t>$\rho_{alb} \quad (tonf/m^3)$</t>
   </si>
   <si>
@@ -333,17 +294,57 @@
   </si>
   <si>
     <t>N°Hiladas</t>
+  </si>
+  <si>
+    <t>$V_2 $ $ (tonf)$</t>
+  </si>
+  <si>
+    <t>$M_3 $$(tonf \cdot m)$</t>
+  </si>
+  <si>
+    <t>$d $$ (m)$</t>
+  </si>
+  <si>
+    <t>$\tau_{sol} $$ (tonf/m^2)$</t>
+  </si>
+  <si>
+    <t>$M/Vd$$ (-)$</t>
+  </si>
+  <si>
+    <t>$\tau_{0resist} $ $ (tonf/m^2)$</t>
+  </si>
+  <si>
+    <t>$\tau_{1resist} $ $ (tonf/m^2)$</t>
+  </si>
+  <si>
+    <t>$\rho_h$ $ (-)$</t>
+  </si>
+  <si>
+    <t>$Escantillon $ $ (m)$</t>
+  </si>
+  <si>
+    <t>$A_{esc} $ $ (m^2)$</t>
+  </si>
+  <si>
+    <t>$b $ $ (m)$</t>
+  </si>
+  <si>
+    <t>$f'm $ $ (MPa)$</t>
+  </si>
+  <si>
+    <t>$F_s$ $ (tonf/m^2)$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="181" formatCode="0.00000"/>
     <numFmt numFmtId="183" formatCode="0.E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -587,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -705,6 +706,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1227,48 +1237,48 @@
         <v>0</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="42"/>
       <c r="C4" s="42" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C5" s="39">
         <v>5.6189</v>
@@ -1291,7 +1301,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C6" s="39">
         <v>3.9243999999999999</v>
@@ -1314,7 +1324,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="39" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C7" s="39">
         <v>6.1524000000000001</v>
@@ -1337,7 +1347,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="39" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C8" s="39">
         <v>4.5667999999999997</v>
@@ -1360,7 +1370,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="39" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C9" s="39">
         <v>5.4020999999999999</v>
@@ -1383,7 +1393,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="39" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C10" s="39">
         <v>5.4909999999999997</v>
@@ -1406,7 +1416,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="39" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C11" s="39">
         <v>3.0482</v>
@@ -1429,7 +1439,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C12" s="39">
         <v>5.4813000000000001</v>
@@ -1452,7 +1462,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="39" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C13" s="39">
         <v>3.8298000000000001</v>
@@ -1475,7 +1485,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="39" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C14" s="39">
         <v>2.0876999999999999</v>
@@ -1498,7 +1508,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="39" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C15" s="39">
         <v>1.8138000000000001</v>
@@ -1521,7 +1531,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="39" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C16" s="39">
         <v>2.4049999999999998</v>
@@ -1544,7 +1554,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="39" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C17" s="39">
         <v>5.8376000000000001</v>
@@ -1567,7 +1577,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="39" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C18" s="39">
         <v>1.8027</v>
@@ -1590,7 +1600,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="39" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C19" s="39">
         <v>2.8479999999999999</v>
@@ -1613,7 +1623,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="39" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C20" s="39">
         <v>3.8689</v>
@@ -1636,7 +1646,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="39" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C21" s="39">
         <v>0.60199999999999998</v>
@@ -1659,7 +1669,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="39" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C22" s="39">
         <v>2.8382000000000001</v>
@@ -1682,7 +1692,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="39" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C23" s="39">
         <v>3.5468999999999999</v>
@@ -1705,7 +1715,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="39" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C24" s="39">
         <v>3.7900999999999998</v>
@@ -1728,7 +1738,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="39" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C25" s="39">
         <v>3.7988</v>
@@ -1751,7 +1761,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="39" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C26" s="39">
         <v>2.1093999999999999</v>
@@ -1774,7 +1784,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="39" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C27" s="39">
         <v>1.8062</v>
@@ -1797,7 +1807,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="39" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C28" s="39">
         <v>2.4131999999999998</v>
@@ -1820,7 +1830,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="39" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C29" s="39">
         <v>1.9093</v>
@@ -1843,7 +1853,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="39" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C30" s="39">
         <v>4.38</v>
@@ -1866,7 +1876,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="39" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C31" s="39">
         <v>3.0327000000000002</v>
@@ -1889,7 +1899,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="39" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C32" s="39">
         <v>0.81130000000000002</v>
@@ -1912,7 +1922,7 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="39" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C33" s="39">
         <v>3.8149000000000002</v>
@@ -1942,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DECA69-FFD3-42FF-AF12-189361EB5B99}">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="L11" sqref="L10:L11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1961,7 +1971,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="B1" s="22">
         <v>14</v>
@@ -1969,7 +1979,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="B2" s="22">
         <v>0.14000000000000001</v>
@@ -1977,7 +1987,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="B3" s="22">
         <v>17000</v>
@@ -1985,14 +1995,14 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="B4" s="31">
         <f>0.0000139*2</f>
         <v>2.7800000000000001E-5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F4" s="30">
         <v>1.3900000000000001E-5</v>
@@ -2000,7 +2010,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="B5" s="22">
         <v>0.104</v>
@@ -2022,7 +2032,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3">
         <f>MIN(0.13*SQRT(B1),0.28)</f>
@@ -2031,7 +2041,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3">
         <f>MIN(0.06*SQRT(B1),0.19)</f>
@@ -2040,12 +2050,12 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3">
         <f>MIN(0.17*SQRT(B1),0.84)</f>
@@ -2054,7 +2064,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3">
         <f>MIN(0.13*SQRT(B1),0.52)</f>
@@ -2066,34 +2076,34 @@
         <v>0</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>2</v>
@@ -3030,7 +3040,7 @@
         <v>3</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3575,40 +3585,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CAD58B-62DD-49B0-8FF5-2F3E018E2753}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.5546875" style="6"/>
     <col min="3" max="4" width="20.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5546875" style="6"/>
-    <col min="7" max="8" width="20.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="6"/>
+    <col min="5" max="5" width="11.5546875" style="6"/>
+    <col min="6" max="6" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.5546875" style="6"/>
+    <col min="15" max="16" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" style="6"/>
+    <col min="19" max="19" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
     </row>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="37" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" s="35" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C4" s="33">
         <f>'Resistencia al corte'!B9</f>
@@ -3619,9 +3640,9 @@
         <v>0.63608175575157011</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C5" s="34">
         <f>'Resistencia al corte'!B10</f>
@@ -3632,8 +3653,1305 @@
         <v>0.48641546028061239</v>
       </c>
     </row>
+    <row r="8" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+    </row>
+    <row r="9" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="37" t="str">
+        <f>'Resistencia al corte'!A16</f>
+        <v>Pier</v>
+      </c>
+      <c r="G9" s="37" t="str">
+        <f>'Resistencia al corte'!B16</f>
+        <v>$V_2 $ $ (tonf)$</v>
+      </c>
+      <c r="H9" s="37" t="str">
+        <f>'Resistencia al corte'!C16</f>
+        <v>$M_3 $$(tonf \cdot m)$</v>
+      </c>
+      <c r="I9" s="37" t="str">
+        <f>'Resistencia al corte'!D16</f>
+        <v>$d $$ (m)$</v>
+      </c>
+      <c r="J9" s="37" t="str">
+        <f>'Resistencia al corte'!E16</f>
+        <v>$\tau_{sol} $$ (tonf/m^2)$</v>
+      </c>
+      <c r="K9" s="37" t="str">
+        <f>'Resistencia al corte'!F16</f>
+        <v>$M/Vd$$ (-)$</v>
+      </c>
+      <c r="N9" s="37" t="str">
+        <f t="shared" ref="N9:N38" si="0">F9</f>
+        <v>Pier</v>
+      </c>
+      <c r="O9" s="37" t="str">
+        <f>'Resistencia al corte'!G16</f>
+        <v>$\tau_{0resist} $ $ (tonf/m^2)$</v>
+      </c>
+      <c r="P9" s="37" t="str">
+        <f>'Resistencia al corte'!H16</f>
+        <v>$\tau_{1resist} $ $ (tonf/m^2)$</v>
+      </c>
+      <c r="Q9" s="37" t="str">
+        <f>'Resistencia al corte'!I16</f>
+        <v>$\rho_h$ $ (-)$</v>
+      </c>
+      <c r="S9" s="46" t="str">
+        <f>'Resistencia al corte'!A2</f>
+        <v>$b $ $ (m)$</v>
+      </c>
+      <c r="T9" s="7">
+        <f>'Resistencia al corte'!B2</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F10" s="6" t="str">
+        <f>'Resistencia al corte'!A17</f>
+        <v>M1Y</v>
+      </c>
+      <c r="G10" s="25">
+        <f>'Resistencia al corte'!B17</f>
+        <v>1.6123000000000001</v>
+      </c>
+      <c r="H10" s="25">
+        <f>'Resistencia al corte'!C17</f>
+        <v>1.8597999999999999</v>
+      </c>
+      <c r="I10" s="6">
+        <f>'Resistencia al corte'!D17</f>
+        <v>3.9</v>
+      </c>
+      <c r="J10" s="25">
+        <f>'Resistencia al corte'!E17</f>
+        <v>2.9529304029304027</v>
+      </c>
+      <c r="K10" s="25">
+        <f>'Resistencia al corte'!F17</f>
+        <v>0.29577113122359039</v>
+      </c>
+      <c r="N10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M1Y</v>
+      </c>
+      <c r="O10" s="25">
+        <f>'Resistencia al corte'!G17</f>
+        <v>25.338059818987691</v>
+      </c>
+      <c r="P10" s="25">
+        <f>'Resistencia al corte'!H17</f>
+        <v>59.181478623408083</v>
+      </c>
+      <c r="Q10" s="44">
+        <f>'Resistencia al corte'!I17</f>
+        <v>1.9107196724843785E-4</v>
+      </c>
+      <c r="S10" s="46" t="str">
+        <f>'Resistencia al corte'!A4</f>
+        <v>$A_{esc} $ $ (m^2)$</v>
+      </c>
+      <c r="T10" s="7">
+        <f>'Resistencia al corte'!B4</f>
+        <v>2.7800000000000001E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F11" s="6" t="str">
+        <f>'Resistencia al corte'!A18</f>
+        <v>M2Y</v>
+      </c>
+      <c r="G11" s="25">
+        <f>'Resistencia al corte'!B18</f>
+        <v>0.89359999999999995</v>
+      </c>
+      <c r="H11" s="25">
+        <f>'Resistencia al corte'!C18</f>
+        <v>0.61270000000000002</v>
+      </c>
+      <c r="I11" s="6">
+        <f>'Resistencia al corte'!D18</f>
+        <v>2.25</v>
+      </c>
+      <c r="J11" s="25">
+        <f>'Resistencia al corte'!E18</f>
+        <v>2.8368253968253963</v>
+      </c>
+      <c r="K11" s="25">
+        <f>'Resistencia al corte'!F18</f>
+        <v>0.3047349050034816</v>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M2Y</v>
+      </c>
+      <c r="O11" s="25">
+        <f>'Resistencia al corte'!G18</f>
+        <v>25.257385854968668</v>
+      </c>
+      <c r="P11" s="25">
+        <f>'Resistencia al corte'!H18</f>
+        <v>59.047321141900476</v>
+      </c>
+      <c r="Q11" s="44">
+        <f>'Resistencia al corte'!I18</f>
+        <v>1.8355929038281981E-4</v>
+      </c>
+      <c r="S11" s="46" t="str">
+        <f>'Resistencia al corte'!A5</f>
+        <v>$Escantillon $ $ (m)$</v>
+      </c>
+      <c r="T11" s="7">
+        <f>'Resistencia al corte'!B5</f>
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F12" s="6" t="str">
+        <f>'Resistencia al corte'!A19</f>
+        <v>M3Y</v>
+      </c>
+      <c r="G12" s="25">
+        <f>'Resistencia al corte'!B19</f>
+        <v>1.6081000000000001</v>
+      </c>
+      <c r="H12" s="25">
+        <f>'Resistencia al corte'!C19</f>
+        <v>1.9031</v>
+      </c>
+      <c r="I12" s="6">
+        <f>'Resistencia al corte'!D19</f>
+        <v>3.9</v>
+      </c>
+      <c r="J12" s="25">
+        <f>'Resistencia al corte'!E19</f>
+        <v>2.9452380952380954</v>
+      </c>
+      <c r="K12" s="25">
+        <f>'Resistencia al corte'!F19</f>
+        <v>0.30344777002323176</v>
+      </c>
+      <c r="N12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M3Y</v>
+      </c>
+      <c r="O12" s="25">
+        <f>'Resistencia al corte'!G19</f>
+        <v>25.268970069790914</v>
+      </c>
+      <c r="P12" s="25">
+        <f>'Resistencia al corte'!H19</f>
+        <v>59.066585214326984</v>
+      </c>
+      <c r="Q12" s="44">
+        <f>'Resistencia al corte'!I19</f>
+        <v>1.9057422969187676E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F13" s="6" t="str">
+        <f>'Resistencia al corte'!A20</f>
+        <v>M4Y</v>
+      </c>
+      <c r="G13" s="25">
+        <f>'Resistencia al corte'!B20</f>
+        <v>1.6175999999999999</v>
+      </c>
+      <c r="H13" s="25">
+        <f>'Resistencia al corte'!C20</f>
+        <v>2.5688</v>
+      </c>
+      <c r="I13" s="6">
+        <f>'Resistencia al corte'!D20</f>
+        <v>3.9</v>
+      </c>
+      <c r="J13" s="25">
+        <f>'Resistencia al corte'!E20</f>
+        <v>2.9626373626373623</v>
+      </c>
+      <c r="K13" s="25">
+        <f>'Resistencia al corte'!F20</f>
+        <v>0.40718760303330037</v>
+      </c>
+      <c r="N13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M4Y</v>
+      </c>
+      <c r="O13" s="25">
+        <f>'Resistencia al corte'!G20</f>
+        <v>24.335311572700295</v>
+      </c>
+      <c r="P13" s="25">
+        <f>'Resistencia al corte'!H20</f>
+        <v>57.513949564387715</v>
+      </c>
+      <c r="Q13" s="44">
+        <f>'Resistencia al corte'!I20</f>
+        <v>1.9170006464124111E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F14" s="6" t="str">
+        <f>'Resistencia al corte'!A21</f>
+        <v>M5Y</v>
+      </c>
+      <c r="G14" s="25">
+        <f>'Resistencia al corte'!B21</f>
+        <v>1.4973000000000001</v>
+      </c>
+      <c r="H14" s="25">
+        <f>'Resistencia al corte'!C21</f>
+        <v>2.7553000000000001</v>
+      </c>
+      <c r="I14" s="6">
+        <f>'Resistencia al corte'!D21</f>
+        <v>3.9</v>
+      </c>
+      <c r="J14" s="25">
+        <f>'Resistencia al corte'!E21</f>
+        <v>2.7423076923076923</v>
+      </c>
+      <c r="K14" s="25">
+        <f>'Resistencia al corte'!F21</f>
+        <v>0.47184076637092065</v>
+      </c>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M5Y</v>
+      </c>
+      <c r="O14" s="25">
+        <f>'Resistencia al corte'!G21</f>
+        <v>23.753433102661713</v>
+      </c>
+      <c r="P14" s="25">
+        <f>'Resistencia al corte'!H21</f>
+        <v>56.546309619665678</v>
+      </c>
+      <c r="Q14" s="44">
+        <f>'Resistencia al corte'!I21</f>
+        <v>1.7744343891402717E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F15" s="6" t="str">
+        <f>'Resistencia al corte'!A22</f>
+        <v>M6Y</v>
+      </c>
+      <c r="G15" s="25">
+        <f>'Resistencia al corte'!B22</f>
+        <v>1.9168000000000001</v>
+      </c>
+      <c r="H15" s="25">
+        <f>'Resistencia al corte'!C22</f>
+        <v>2.0171999999999999</v>
+      </c>
+      <c r="I15" s="6">
+        <f>'Resistencia al corte'!D22</f>
+        <v>3.9</v>
+      </c>
+      <c r="J15" s="25">
+        <f>'Resistencia al corte'!E22</f>
+        <v>3.5106227106227106</v>
+      </c>
+      <c r="K15" s="25">
+        <f>'Resistencia al corte'!F22</f>
+        <v>0.269840760241428</v>
+      </c>
+      <c r="N15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M6Y</v>
+      </c>
+      <c r="O15" s="25">
+        <f>'Resistencia al corte'!G22</f>
+        <v>25.571433157827151</v>
+      </c>
+      <c r="P15" s="25">
+        <f>'Resistencia al corte'!H22</f>
+        <v>59.569568879916865</v>
+      </c>
+      <c r="Q15" s="44">
+        <f>'Resistencia al corte'!I22</f>
+        <v>2.2715794009911658E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="F16" s="6" t="str">
+        <f>'Resistencia al corte'!A23</f>
+        <v>M7Y</v>
+      </c>
+      <c r="G16" s="25">
+        <f>'Resistencia al corte'!B23</f>
+        <v>1.1177999999999999</v>
+      </c>
+      <c r="H16" s="25">
+        <f>'Resistencia al corte'!C23</f>
+        <v>0.82740000000000002</v>
+      </c>
+      <c r="I16" s="6">
+        <f>'Resistencia al corte'!D23</f>
+        <v>2.25</v>
+      </c>
+      <c r="J16" s="25">
+        <f>'Resistencia al corte'!E23</f>
+        <v>3.548571428571428</v>
+      </c>
+      <c r="K16" s="25">
+        <f>'Resistencia al corte'!F23</f>
+        <v>0.32897954315023564</v>
+      </c>
+      <c r="N16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M7Y</v>
+      </c>
+      <c r="O16" s="25">
+        <f>'Resistencia al corte'!G23</f>
+        <v>25.039184111647884</v>
+      </c>
+      <c r="P16" s="25">
+        <f>'Resistencia al corte'!H23</f>
+        <v>58.684460624254633</v>
+      </c>
+      <c r="Q16" s="44">
+        <f>'Resistencia al corte'!I23</f>
+        <v>2.2961344537815123E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F17" s="6" t="str">
+        <f>'Resistencia al corte'!A24</f>
+        <v>M8Y</v>
+      </c>
+      <c r="G17" s="25">
+        <f>'Resistencia al corte'!B24</f>
+        <v>1.9679</v>
+      </c>
+      <c r="H17" s="25">
+        <f>'Resistencia al corte'!C24</f>
+        <v>1.9932000000000001</v>
+      </c>
+      <c r="I17" s="6">
+        <f>'Resistencia al corte'!D24</f>
+        <v>3.9</v>
+      </c>
+      <c r="J17" s="25">
+        <f>'Resistencia al corte'!E24</f>
+        <v>3.6042124542124543</v>
+      </c>
+      <c r="K17" s="25">
+        <f>'Resistencia al corte'!F24</f>
+        <v>0.25970675495549728</v>
+      </c>
+      <c r="N17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M8Y</v>
+      </c>
+      <c r="O17" s="25">
+        <f>'Resistencia al corte'!G24</f>
+        <v>25.662639205400527</v>
+      </c>
+      <c r="P17" s="25">
+        <f>'Resistencia al corte'!H24</f>
+        <v>59.721240782859709</v>
+      </c>
+      <c r="Q17" s="44">
+        <f>'Resistencia al corte'!I24</f>
+        <v>2.3321374703727648E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F18" s="6" t="str">
+        <f>'Resistencia al corte'!A25</f>
+        <v>M1X</v>
+      </c>
+      <c r="G18" s="25">
+        <f>'Resistencia al corte'!B25</f>
+        <v>1.5024999999999999</v>
+      </c>
+      <c r="H18" s="25">
+        <f>'Resistencia al corte'!C25</f>
+        <v>1.0904</v>
+      </c>
+      <c r="I18" s="6">
+        <f>'Resistencia al corte'!D25</f>
+        <v>3.3</v>
+      </c>
+      <c r="J18" s="25">
+        <f>'Resistencia al corte'!E25</f>
+        <v>3.252164502164502</v>
+      </c>
+      <c r="K18" s="25">
+        <f>'Resistencia al corte'!F25</f>
+        <v>0.21991630111430446</v>
+      </c>
+      <c r="N18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M1X</v>
+      </c>
+      <c r="O18" s="25">
+        <f>'Resistencia al corte'!G25</f>
+        <v>26.02075328997126</v>
+      </c>
+      <c r="P18" s="25">
+        <f>'Resistencia al corte'!H25</f>
+        <v>60.316769765011649</v>
+      </c>
+      <c r="Q18" s="44">
+        <f>'Resistencia al corte'!I25</f>
+        <v>2.1043417366946782E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F19" s="6" t="str">
+        <f>'Resistencia al corte'!A26</f>
+        <v>M2X</v>
+      </c>
+      <c r="G19" s="25">
+        <f>'Resistencia al corte'!B26</f>
+        <v>0.70140000000000002</v>
+      </c>
+      <c r="H19" s="25">
+        <f>'Resistencia al corte'!C26</f>
+        <v>0.5968</v>
+      </c>
+      <c r="I19" s="6">
+        <f>'Resistencia al corte'!D26</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J19" s="25">
+        <f>'Resistencia al corte'!E26</f>
+        <v>4.4732142857142847</v>
+      </c>
+      <c r="K19" s="25">
+        <f>'Resistencia al corte'!F26</f>
+        <v>0.75970507963664491</v>
+      </c>
+      <c r="N19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M2X</v>
+      </c>
+      <c r="O19" s="25">
+        <f>'Resistencia al corte'!G26</f>
+        <v>21.162654283270196</v>
+      </c>
+      <c r="P19" s="25">
+        <f>'Resistencia al corte'!H26</f>
+        <v>52.237951083188449</v>
+      </c>
+      <c r="Q19" s="44">
+        <f>'Resistencia al corte'!I26</f>
+        <v>2.894432773109244E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F20" s="6" t="str">
+        <f>'Resistencia al corte'!A27</f>
+        <v>M3X</v>
+      </c>
+      <c r="G20" s="25">
+        <f>'Resistencia al corte'!B27</f>
+        <v>0.73409999999999997</v>
+      </c>
+      <c r="H20" s="25">
+        <f>'Resistencia al corte'!C27</f>
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I20" s="6">
+        <f>'Resistencia al corte'!D27</f>
+        <v>0.98</v>
+      </c>
+      <c r="J20" s="25">
+        <f>'Resistencia al corte'!E27</f>
+        <v>5.3505830903790077</v>
+      </c>
+      <c r="K20" s="25">
+        <f>'Resistencia al corte'!F27</f>
+        <v>0.67693607888598839</v>
+      </c>
+      <c r="N20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M3X</v>
+      </c>
+      <c r="O20" s="25">
+        <f>'Resistencia al corte'!G27</f>
+        <v>21.907575290026106</v>
+      </c>
+      <c r="P20" s="25">
+        <f>'Resistencia al corte'!H27</f>
+        <v>53.47672405540682</v>
+      </c>
+      <c r="Q20" s="44">
+        <f>'Resistencia al corte'!I27</f>
+        <v>3.4621419996570059E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F21" s="6" t="str">
+        <f>'Resistencia al corte'!A28</f>
+        <v>M4X</v>
+      </c>
+      <c r="G21" s="25">
+        <f>'Resistencia al corte'!B28</f>
+        <v>1.4292</v>
+      </c>
+      <c r="H21" s="25">
+        <f>'Resistencia al corte'!C28</f>
+        <v>1.3167</v>
+      </c>
+      <c r="I21" s="6">
+        <f>'Resistencia al corte'!D28</f>
+        <v>3.3</v>
+      </c>
+      <c r="J21" s="25">
+        <f>'Resistencia al corte'!E28</f>
+        <v>3.0935064935064935</v>
+      </c>
+      <c r="K21" s="25">
+        <f>'Resistencia al corte'!F28</f>
+        <v>0.27917716204869858</v>
+      </c>
+      <c r="N21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M4X</v>
+      </c>
+      <c r="O21" s="25">
+        <f>'Resistencia al corte'!G28</f>
+        <v>25.487405541561714</v>
+      </c>
+      <c r="P21" s="25">
+        <f>'Resistencia al corte'!H28</f>
+        <v>59.429834412764613</v>
+      </c>
+      <c r="Q21" s="44">
+        <f>'Resistencia al corte'!I28</f>
+        <v>2.0016806722689077E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F22" s="6" t="str">
+        <f>'Resistencia al corte'!A29</f>
+        <v>M5X</v>
+      </c>
+      <c r="G22" s="25">
+        <f>'Resistencia al corte'!B29</f>
+        <v>1.7835000000000001</v>
+      </c>
+      <c r="H22" s="25">
+        <f>'Resistencia al corte'!C29</f>
+        <v>2.2806999999999999</v>
+      </c>
+      <c r="I22" s="6">
+        <f>'Resistencia al corte'!D29</f>
+        <v>3.82</v>
+      </c>
+      <c r="J22" s="25">
+        <f>'Resistencia al corte'!E29</f>
+        <v>3.3348915482423336</v>
+      </c>
+      <c r="K22" s="25">
+        <f>'Resistencia al corte'!F29</f>
+        <v>0.33475855610695482</v>
+      </c>
+      <c r="N22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M5X</v>
+      </c>
+      <c r="O22" s="25">
+        <f>'Resistencia al corte'!G29</f>
+        <v>24.987172995037412</v>
+      </c>
+      <c r="P22" s="25">
+        <f>'Resistencia al corte'!H29</f>
+        <v>58.597968278183544</v>
+      </c>
+      <c r="Q22" s="44">
+        <f>'Resistencia al corte'!I29</f>
+        <v>2.1578710018038631E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F23" s="6" t="str">
+        <f>'Resistencia al corte'!A30</f>
+        <v>M6X</v>
+      </c>
+      <c r="G23" s="25">
+        <f>'Resistencia al corte'!B30</f>
+        <v>0.66049999999999998</v>
+      </c>
+      <c r="H23" s="25">
+        <f>'Resistencia al corte'!C30</f>
+        <v>0.43880000000000002</v>
+      </c>
+      <c r="I23" s="6">
+        <f>'Resistencia al corte'!D30</f>
+        <v>0.98</v>
+      </c>
+      <c r="J23" s="25">
+        <f>'Resistencia al corte'!E30</f>
+        <v>4.8141399416909616</v>
+      </c>
+      <c r="K23" s="25">
+        <f>'Resistencia al corte'!F30</f>
+        <v>0.67790325819957065</v>
+      </c>
+      <c r="N23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M6X</v>
+      </c>
+      <c r="O23" s="25">
+        <f>'Resistencia al corte'!G30</f>
+        <v>21.898870676203867</v>
+      </c>
+      <c r="P23" s="25">
+        <f>'Resistencia al corte'!H30</f>
+        <v>53.462248640914822</v>
+      </c>
+      <c r="Q23" s="44">
+        <f>'Resistencia al corte'!I30</f>
+        <v>3.1150317269765048E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F24" s="6" t="str">
+        <f>'Resistencia al corte'!A31</f>
+        <v>M7X</v>
+      </c>
+      <c r="G24" s="25">
+        <f>'Resistencia al corte'!B31</f>
+        <v>1.0144</v>
+      </c>
+      <c r="H24" s="25">
+        <f>'Resistencia al corte'!C31</f>
+        <v>0.79590000000000005</v>
+      </c>
+      <c r="I24" s="6">
+        <f>'Resistencia al corte'!D31</f>
+        <v>1.64</v>
+      </c>
+      <c r="J24" s="25">
+        <f>'Resistencia al corte'!E31</f>
+        <v>4.4181184668989539</v>
+      </c>
+      <c r="K24" s="25">
+        <f>'Resistencia al corte'!F31</f>
+        <v>0.47841569208278845</v>
+      </c>
+      <c r="N24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M7X</v>
+      </c>
+      <c r="O24" s="25">
+        <f>'Resistencia al corte'!G31</f>
+        <v>23.694258771254905</v>
+      </c>
+      <c r="P24" s="25">
+        <f>'Resistencia al corte'!H31</f>
+        <v>56.447905142236479</v>
+      </c>
+      <c r="Q24" s="44">
+        <f>'Resistencia al corte'!I31</f>
+        <v>2.8587825374052066E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F25" s="6" t="str">
+        <f>'Resistencia al corte'!A32</f>
+        <v>M8X</v>
+      </c>
+      <c r="G25" s="25">
+        <f>'Resistencia al corte'!B32</f>
+        <v>1.8542000000000001</v>
+      </c>
+      <c r="H25" s="25">
+        <f>'Resistencia al corte'!C32</f>
+        <v>1.5748</v>
+      </c>
+      <c r="I25" s="6">
+        <f>'Resistencia al corte'!D32</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J25" s="25">
+        <f>'Resistencia al corte'!E32</f>
+        <v>2.5969187675070029</v>
+      </c>
+      <c r="K25" s="25">
+        <f>'Resistencia al corte'!F32</f>
+        <v>0.16653236637120603</v>
+      </c>
+      <c r="N25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M8X</v>
+      </c>
+      <c r="O25" s="25">
+        <f>'Resistencia al corte'!G32</f>
+        <v>26.501208702659145</v>
+      </c>
+      <c r="P25" s="25">
+        <f>'Resistencia al corte'!H32</f>
+        <v>61.115747340077945</v>
+      </c>
+      <c r="Q25" s="44">
+        <f>'Resistencia al corte'!I32</f>
+        <v>1.6803592025045315E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F26" s="6" t="str">
+        <f>'Resistencia al corte'!A33</f>
+        <v>M9X</v>
+      </c>
+      <c r="G26" s="25">
+        <f>'Resistencia al corte'!B33</f>
+        <v>0.121</v>
+      </c>
+      <c r="H26" s="25">
+        <f>'Resistencia al corte'!C33</f>
+        <v>0.1002</v>
+      </c>
+      <c r="I26" s="6">
+        <f>'Resistencia al corte'!D33</f>
+        <v>0.37</v>
+      </c>
+      <c r="J26" s="25">
+        <f>'Resistencia al corte'!E33</f>
+        <v>2.3359073359073355</v>
+      </c>
+      <c r="K26" s="25">
+        <f>'Resistencia al corte'!F33</f>
+        <v>2.238105874469511</v>
+      </c>
+      <c r="N26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M9X</v>
+      </c>
+      <c r="O26" s="25">
+        <f>'Resistencia al corte'!G33</f>
+        <v>19</v>
+      </c>
+      <c r="P26" s="25">
+        <f>'Resistencia al corte'!H33</f>
+        <v>48.641546028061242</v>
+      </c>
+      <c r="Q26" s="44">
+        <f>'Resistencia al corte'!I33</f>
+        <v>1.5114694526459233E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F27" s="6" t="str">
+        <f>'Resistencia al corte'!A34</f>
+        <v>M10X</v>
+      </c>
+      <c r="G27" s="25">
+        <f>'Resistencia al corte'!B34</f>
+        <v>1.3111999999999999</v>
+      </c>
+      <c r="H27" s="25">
+        <f>'Resistencia al corte'!C34</f>
+        <v>1.6113</v>
+      </c>
+      <c r="I27" s="6">
+        <f>'Resistencia al corte'!D34</f>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J27" s="25">
+        <f>'Resistencia al corte'!E34</f>
+        <v>4.0369458128078817</v>
+      </c>
+      <c r="K27" s="25">
+        <f>'Resistencia al corte'!F34</f>
+        <v>0.52968720414045567</v>
+      </c>
+      <c r="N27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M10X</v>
+      </c>
+      <c r="O27" s="25">
+        <f>'Resistencia al corte'!G34</f>
+        <v>23.2328151627359</v>
+      </c>
+      <c r="P27" s="25">
+        <f>'Resistencia al corte'!H34</f>
+        <v>55.680543414949909</v>
+      </c>
+      <c r="Q27" s="44">
+        <f>'Resistencia al corte'!I34</f>
+        <v>2.6121414082874532E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F28" s="6" t="str">
+        <f>'Resistencia al corte'!A35</f>
+        <v>M11X</v>
+      </c>
+      <c r="G28" s="25">
+        <f>'Resistencia al corte'!B35</f>
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="H28" s="25">
+        <f>'Resistencia al corte'!C35</f>
+        <v>2.3294999999999999</v>
+      </c>
+      <c r="I28" s="6">
+        <f>'Resistencia al corte'!D35</f>
+        <v>2.77</v>
+      </c>
+      <c r="J28" s="25">
+        <f>'Resistencia al corte'!E35</f>
+        <v>4.0278494069107786</v>
+      </c>
+      <c r="K28" s="25">
+        <f>'Resistencia al corte'!F35</f>
+        <v>0.53839611347111216</v>
+      </c>
+      <c r="N28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M11X</v>
+      </c>
+      <c r="O28" s="25">
+        <f>'Resistencia al corte'!G35</f>
+        <v>23.154434978759991</v>
+      </c>
+      <c r="P28" s="25">
+        <f>'Resistencia al corte'!H35</f>
+        <v>55.550200395238733</v>
+      </c>
+      <c r="Q28" s="44">
+        <f>'Resistencia al corte'!I35</f>
+        <v>2.6062554985893275E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F29" s="6" t="str">
+        <f>'Resistencia al corte'!A36</f>
+        <v>M12X</v>
+      </c>
+      <c r="G29" s="25">
+        <f>'Resistencia al corte'!B36</f>
+        <v>2.8323999999999998</v>
+      </c>
+      <c r="H29" s="25">
+        <f>'Resistencia al corte'!C36</f>
+        <v>3.9697</v>
+      </c>
+      <c r="I29" s="6">
+        <f>'Resistencia al corte'!D36</f>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J29" s="25">
+        <f>'Resistencia al corte'!E36</f>
+        <v>8.720443349753694</v>
+      </c>
+      <c r="K29" s="25">
+        <f>'Resistencia al corte'!F36</f>
+        <v>0.60410873683339106</v>
+      </c>
+      <c r="N29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M12X</v>
+      </c>
+      <c r="O29" s="25">
+        <f>'Resistencia al corte'!G36</f>
+        <v>22.563021368499481</v>
+      </c>
+      <c r="P29" s="25">
+        <f>'Resistencia al corte'!H36</f>
+        <v>54.566703904807682</v>
+      </c>
+      <c r="Q29" s="44">
+        <f>'Resistencia al corte'!I36</f>
+        <v>5.6426398145465091E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F30" s="6" t="str">
+        <f>'Resistencia al corte'!A37</f>
+        <v>M13X</v>
+      </c>
+      <c r="G30" s="25">
+        <f>'Resistencia al corte'!B37</f>
+        <v>1.6707000000000001</v>
+      </c>
+      <c r="H30" s="25">
+        <f>'Resistencia al corte'!C37</f>
+        <v>1.1577999999999999</v>
+      </c>
+      <c r="I30" s="6">
+        <f>'Resistencia al corte'!D37</f>
+        <v>3.3</v>
+      </c>
+      <c r="J30" s="25">
+        <f>'Resistencia al corte'!E37</f>
+        <v>3.616233766233766</v>
+      </c>
+      <c r="K30" s="25">
+        <f>'Resistencia al corte'!F37</f>
+        <v>0.21000088875829584</v>
+      </c>
+      <c r="N30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M13X</v>
+      </c>
+      <c r="O30" s="25">
+        <f>'Resistencia al corte'!G37</f>
+        <v>26.109992001175343</v>
+      </c>
+      <c r="P30" s="25">
+        <f>'Resistencia al corte'!H37</f>
+        <v>60.465170068550734</v>
+      </c>
+      <c r="Q30" s="44">
+        <f>'Resistencia al corte'!I37</f>
+        <v>2.3399159663865549E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F31" s="6" t="str">
+        <f>'Resistencia al corte'!A38</f>
+        <v>M14X</v>
+      </c>
+      <c r="G31" s="25">
+        <f>'Resistencia al corte'!B38</f>
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="H31" s="25">
+        <f>'Resistencia al corte'!C38</f>
+        <v>0.62360000000000004</v>
+      </c>
+      <c r="I31" s="6">
+        <f>'Resistencia al corte'!D38</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J31" s="25">
+        <f>'Resistencia al corte'!E38</f>
+        <v>4.8418367346938771</v>
+      </c>
+      <c r="K31" s="25">
+        <f>'Resistencia al corte'!F38</f>
+        <v>0.73338476591901247</v>
+      </c>
+      <c r="N31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M14X</v>
+      </c>
+      <c r="O31" s="25">
+        <f>'Resistencia al corte'!G38</f>
+        <v>21.399537106728889</v>
+      </c>
+      <c r="P31" s="25">
+        <f>'Resistencia al corte'!H38</f>
+        <v>52.631877468163601</v>
+      </c>
+      <c r="Q31" s="44">
+        <f>'Resistencia al corte'!I38</f>
+        <v>3.1329531812725089E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F32" s="6" t="str">
+        <f>'Resistencia al corte'!A39</f>
+        <v>M15X</v>
+      </c>
+      <c r="G32" s="25">
+        <f>'Resistencia al corte'!B39</f>
+        <v>0.74350000000000005</v>
+      </c>
+      <c r="H32" s="25">
+        <f>'Resistencia al corte'!C39</f>
+        <v>0.49080000000000001</v>
+      </c>
+      <c r="I32" s="6">
+        <f>'Resistencia al corte'!D39</f>
+        <v>0.98</v>
+      </c>
+      <c r="J32" s="25">
+        <f>'Resistencia al corte'!E39</f>
+        <v>5.4190962099125359</v>
+      </c>
+      <c r="K32" s="25">
+        <f>'Resistencia al corte'!F39</f>
+        <v>0.67359290723686926</v>
+      </c>
+      <c r="N32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M15X</v>
+      </c>
+      <c r="O32" s="25">
+        <f>'Resistencia al corte'!G39</f>
+        <v>21.937663834868175</v>
+      </c>
+      <c r="P32" s="25">
+        <f>'Resistencia al corte'!H39</f>
+        <v>53.526760066991542</v>
+      </c>
+      <c r="Q32" s="44">
+        <f>'Resistencia al corte'!I39</f>
+        <v>3.5064740181787004E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F33" s="6" t="str">
+        <f>'Resistencia al corte'!A40</f>
+        <v>M16X</v>
+      </c>
+      <c r="G33" s="25">
+        <f>'Resistencia al corte'!B40</f>
+        <v>1.3024</v>
+      </c>
+      <c r="H33" s="25">
+        <f>'Resistencia al corte'!C40</f>
+        <v>1.2633000000000001</v>
+      </c>
+      <c r="I33" s="6">
+        <f>'Resistencia al corte'!D40</f>
+        <v>3.3</v>
+      </c>
+      <c r="J33" s="25">
+        <f>'Resistencia al corte'!E40</f>
+        <v>2.8190476190476188</v>
+      </c>
+      <c r="K33" s="25">
+        <f>'Resistencia al corte'!F40</f>
+        <v>0.29393287916015193</v>
+      </c>
+      <c r="N33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M16X</v>
+      </c>
+      <c r="O33" s="25">
+        <f>'Resistencia al corte'!G40</f>
+        <v>25.354604087558634</v>
+      </c>
+      <c r="P33" s="25">
+        <f>'Resistencia al corte'!H40</f>
+        <v>59.208991061055748</v>
+      </c>
+      <c r="Q33" s="44">
+        <f>'Resistencia al corte'!I40</f>
+        <v>1.8240896358543419E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F34" s="6" t="str">
+        <f>'Resistencia al corte'!A41</f>
+        <v>M17X</v>
+      </c>
+      <c r="G34" s="25">
+        <f>'Resistencia al corte'!B41</f>
+        <v>0.66969999999999996</v>
+      </c>
+      <c r="H34" s="25">
+        <f>'Resistencia al corte'!C41</f>
+        <v>0.44369999999999998</v>
+      </c>
+      <c r="I34" s="6">
+        <f>'Resistencia al corte'!D41</f>
+        <v>0.97</v>
+      </c>
+      <c r="J34" s="25">
+        <f>'Resistencia al corte'!E41</f>
+        <v>4.9315169366715752</v>
+      </c>
+      <c r="K34" s="25">
+        <f>'Resistencia al corte'!F41</f>
+        <v>0.68302625117570726</v>
+      </c>
+      <c r="N34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M17X</v>
+      </c>
+      <c r="O34" s="25">
+        <f>'Resistencia al corte'!G41</f>
+        <v>21.852763739418634</v>
+      </c>
+      <c r="P34" s="25">
+        <f>'Resistencia al corte'!H41</f>
+        <v>53.38557470286861</v>
+      </c>
+      <c r="Q34" s="44">
+        <f>'Resistencia al corte'!I41</f>
+        <v>3.1909815472580788E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F35" s="6" t="str">
+        <f>'Resistencia al corte'!A42</f>
+        <v>M18X</v>
+      </c>
+      <c r="G35" s="25">
+        <f>'Resistencia al corte'!B42</f>
+        <v>1.4371</v>
+      </c>
+      <c r="H35" s="25">
+        <f>'Resistencia al corte'!C42</f>
+        <v>2.4371</v>
+      </c>
+      <c r="I35" s="6">
+        <f>'Resistencia al corte'!D42</f>
+        <v>3.22</v>
+      </c>
+      <c r="J35" s="25">
+        <f>'Resistencia al corte'!E42</f>
+        <v>3.1878881987577636</v>
+      </c>
+      <c r="K35" s="25">
+        <f>'Resistencia al corte'!F42</f>
+        <v>0.52666018651260671</v>
+      </c>
+      <c r="N35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M18X</v>
+      </c>
+      <c r="O35" s="25">
+        <f>'Resistencia al corte'!G42</f>
+        <v>23.260058321386541</v>
+      </c>
+      <c r="P35" s="25">
+        <f>'Resistencia al corte'!H42</f>
+        <v>55.72584766641846</v>
+      </c>
+      <c r="Q35" s="44">
+        <f>'Resistencia al corte'!I42</f>
+        <v>2.0627511874314947E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F36" s="6" t="str">
+        <f>'Resistencia al corte'!A43</f>
+        <v>M19X</v>
+      </c>
+      <c r="G36" s="25">
+        <f>'Resistencia al corte'!B43</f>
+        <v>1.1617999999999999</v>
+      </c>
+      <c r="H36" s="25">
+        <f>'Resistencia al corte'!C43</f>
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="I36" s="6">
+        <f>'Resistencia al corte'!D43</f>
+        <v>1.64</v>
+      </c>
+      <c r="J36" s="25">
+        <f>'Resistencia al corte'!E43</f>
+        <v>5.0601045296167237</v>
+      </c>
+      <c r="K36" s="25">
+        <f>'Resistencia al corte'!F43</f>
+        <v>0.40806108267658686</v>
+      </c>
+      <c r="N36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M19X</v>
+      </c>
+      <c r="O36" s="25">
+        <f>'Resistencia al corte'!G43</f>
+        <v>24.327450255910719</v>
+      </c>
+      <c r="P36" s="25">
+        <f>'Resistencia al corte'!H43</f>
+        <v>57.50087651814971</v>
+      </c>
+      <c r="Q36" s="44">
+        <f>'Resistencia al corte'!I43</f>
+        <v>3.2741852838696461E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F37" s="6" t="str">
+        <f>'Resistencia al corte'!A44</f>
+        <v>M20X</v>
+      </c>
+      <c r="G37" s="25">
+        <f>'Resistencia al corte'!B44</f>
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="H37" s="25">
+        <f>'Resistencia al corte'!C44</f>
+        <v>0.1595</v>
+      </c>
+      <c r="I37" s="6">
+        <f>'Resistencia al corte'!D44</f>
+        <v>0.37</v>
+      </c>
+      <c r="J37" s="25">
+        <f>'Resistencia al corte'!E44</f>
+        <v>4.6389961389961387</v>
+      </c>
+      <c r="K37" s="25">
+        <f>'Resistencia al corte'!F44</f>
+        <v>1.7939287602208951</v>
+      </c>
+      <c r="N37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>M20X</v>
+      </c>
+      <c r="O37" s="25">
+        <f>'Resistencia al corte'!G44</f>
+        <v>19</v>
+      </c>
+      <c r="P37" s="25">
+        <f>'Resistencia al corte'!H44</f>
+        <v>48.641546028061242</v>
+      </c>
+      <c r="Q37" s="44">
+        <f>'Resistencia al corte'!I44</f>
+        <v>3.001703384056325E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="6:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="36" t="str">
+        <f>'Resistencia al corte'!A45</f>
+        <v>M21X</v>
+      </c>
+      <c r="G38" s="34">
+        <f>'Resistencia al corte'!B45</f>
+        <v>1.9393</v>
+      </c>
+      <c r="H38" s="34">
+        <f>'Resistencia al corte'!C45</f>
+        <v>2.0179999999999998</v>
+      </c>
+      <c r="I38" s="36">
+        <f>'Resistencia al corte'!D45</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J38" s="34">
+        <f>'Resistencia al corte'!E45</f>
+        <v>2.7161064425770305</v>
+      </c>
+      <c r="K38" s="34">
+        <f>'Resistencia al corte'!F45</f>
+        <v>0.20403561826937755</v>
+      </c>
+      <c r="N38" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>M21X</v>
+      </c>
+      <c r="O38" s="34">
+        <f>'Resistencia al corte'!G45</f>
+        <v>26.163679435575602</v>
+      </c>
+      <c r="P38" s="34">
+        <f>'Resistencia al corte'!H45</f>
+        <v>60.554450062106589</v>
+      </c>
+      <c r="Q38" s="45">
+        <f>'Resistencia al corte'!I45</f>
+        <v>1.7574806393145495E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3654,13 +4972,13 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C2" s="26"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C3" s="7">
         <v>1.8</v>
@@ -3668,7 +4986,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7">
         <v>0.14000000000000001</v>
@@ -3676,7 +4994,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C5" s="7">
         <v>1.04</v>
@@ -3684,7 +5002,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7">
         <v>10</v>
@@ -3692,13 +5010,13 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C8" s="26"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>2.5</v>
@@ -3706,7 +5024,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7">
         <v>0.14000000000000001</v>
@@ -3714,7 +5032,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C11" s="7">
         <v>0.12</v>
@@ -3722,7 +5040,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>10.49</v>
@@ -3730,7 +5048,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7">
         <f>C3*C4*C5*1000</f>
@@ -3739,7 +5057,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C16" s="7">
         <f>C9*C10*C11*1000</f>
@@ -3748,7 +5066,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C17" s="10">
         <f>C15+C16+'Solicitacion cercha madera'!C27*'Solicitacion cercha madera'!C10/'Solicitación timpano'!C6</f>
@@ -3757,7 +5075,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7">
         <f>'Solicitacion cercha madera'!F22/2*5/C6</f>
@@ -3795,7 +5113,7 @@
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="27" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C2" s="27"/>
       <c r="E2" s="11"/>
@@ -3812,7 +5130,7 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7">
         <v>550</v>
@@ -3831,7 +5149,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7">
         <v>100</v>
@@ -3850,7 +5168,7 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7">
         <v>50</v>
@@ -3897,7 +5215,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7">
         <v>0.157</v>
@@ -3929,7 +5247,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7">
         <v>5</v>
@@ -3948,7 +5266,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>8.5399999999999991</v>
@@ -3967,7 +5285,7 @@
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
         <f>C11*C5/1000*C4/1000</f>
@@ -3987,7 +5305,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C14" s="23">
         <v>4</v>
@@ -3995,7 +5313,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C15" s="7">
         <f>C11/10</f>
@@ -4004,7 +5322,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7">
         <f>C15*C5/1000*C4/1000</f>
@@ -4018,11 +5336,11 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C19" s="27"/>
       <c r="E19" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F19" s="25">
         <f>8.4/5*10/6</f>
@@ -4035,7 +5353,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C20" s="7">
         <f>C3*C8/2</f>
@@ -4048,7 +5366,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C21" s="24">
         <f>$C$16*$C$3*2*5/2</f>
@@ -4057,14 +5375,14 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C22" s="24">
         <f>C16*C3*5/2</f>
         <v>5.871249999999999</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F22" s="24">
         <f>F19*100</f>
@@ -4073,13 +5391,13 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="27" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C25" s="27"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C26" s="24">
         <f>C20+C21</f>
@@ -4088,7 +5406,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C27" s="24">
         <f>C22</f>
@@ -4097,7 +5415,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C28" s="24">
         <f>+F22*6/2</f>

</xml_diff>